<commit_message>
New simulation using cross correlation. Added TF-LUNA docs
</commit_message>
<xml_diff>
--- a/docs/LIDAR/Rain Simulation.xlsx
+++ b/docs/LIDAR/Rain Simulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\johnp\Dropbox\Programming\c++\LIDAR\docs\LIDAR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A683791D-5428-49E1-AC0A-0EDA58BE5614}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7863432D-8C96-4C00-B95D-C8E84097E071}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{6F829C6E-AC9C-4B9E-9DA9-8841D05EEE17}"/>
   </bookViews>
@@ -526,49 +526,49 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>7</c:v>
@@ -886,217 +886,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>3.27</c:v>
+                  <c:v>5.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.43</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.58</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.51</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.64</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="20">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.38</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>3.41</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.38</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.31</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.57</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.41</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.21</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.72</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.88</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.24</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="67">
                   <c:v>3.7</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.45</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.32</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.28</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.23</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.62</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.73</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.61</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.39</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.28</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.62</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.53</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.21</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.41</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.58</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.41</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.37</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.27</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.42</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.46</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.72</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.38</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.39</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.53</c:v>
-                </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="68">
                   <c:v>3.68</c:v>
                 </c:pt>
-                <c:pt idx="49">
-                  <c:v>3.37</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3.71</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>3.78</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3.21</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>3.56</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>3.34</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3.58</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3.34</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>3.31</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3.44</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3.24</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>3.45</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>3.31</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>3.35</c:v>
-                </c:pt>
                 <c:pt idx="69">
-                  <c:v>3.51</c:v>
+                  <c:v>3.52</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3.68</c:v>
+                  <c:v>3.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1354,217 +1354,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>5.1349999999999998</c:v>
+                  <c:v>6.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.4550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5250000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.82</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.93</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.49</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.2149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.2549999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="20">
+                  <c:v>5.8550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.1899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.0949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>5.2050000000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.1899999999999995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.2750000000000004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.38</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.1550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>4.3100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.7350000000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.46</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.2850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.4749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.7149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.93</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.4699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.2050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.81</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.915</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.1050000000000004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.7149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.7149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.9299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.915</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.7450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.07</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.0549999999999997</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.3650000000000002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.6950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.2649999999999997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.6449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.1100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.4050000000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.6449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.96</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.9399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.37</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.12</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.7750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.1850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="67">
                   <c:v>5.35</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.2249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.14</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.1150000000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.15</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.3100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.3650000000000002</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.3049999999999997</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.1950000000000003</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.14</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.3100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5.2649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.1050000000000004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5.2050000000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>5.375</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>5.2050000000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>5.1850000000000005</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.1349999999999998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.71</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.73</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.8600000000000003</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3.88</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.69</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.6950000000000003</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3.835</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.835</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3.84</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>3.6850000000000001</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3.855</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5.38</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5.39</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5.375</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5.1050000000000004</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5.28</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5.17</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.17</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5.1550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5.22</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5.12</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>5.2249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5.1550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>5.25</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>5.38</c:v>
-                </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.1749999999999998</c:v>
+                  <c:v>5.34</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.2549999999999999</c:v>
+                  <c:v>5.26</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.34</c:v>
+                  <c:v>5.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2290,217 +2290,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>5.1349999999999998</c:v>
+                  <c:v>6.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1479999999999997</c:v>
+                  <c:v>5.8660000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1834000000000007</c:v>
+                  <c:v>5.6018000000000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2047200000000009</c:v>
+                  <c:v>5.731440000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2147760000000014</c:v>
+                  <c:v>5.7441520000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2358208000000017</c:v>
+                  <c:v>5.6243216000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2296566400000017</c:v>
+                  <c:v>5.5894572800000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.221725312000002</c:v>
+                  <c:v>5.5945658240000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.232380249600002</c:v>
+                  <c:v>5.4696526592000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.2619041996800018</c:v>
+                  <c:v>5.4657221273600003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2525233597440018</c:v>
+                  <c:v>5.3915777018880009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.2330186877952016</c:v>
+                  <c:v>5.4042621615104007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2564149502361621</c:v>
+                  <c:v>5.4284097292083215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.2501319601889298</c:v>
+                  <c:v>5.3067277833666582</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.2321055681511437</c:v>
+                  <c:v>5.1873822266933267</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.2136844545209158</c:v>
+                  <c:v>5.3359057813546613</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1939475636167334</c:v>
+                  <c:v>5.2847246250837294</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.1851580508933868</c:v>
+                  <c:v>5.3257797000669838</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.2101264407147099</c:v>
+                  <c:v>5.5036237600535873</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2411011525717681</c:v>
+                  <c:v>5.4428990080428701</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.253880922057415</c:v>
+                  <c:v>5.5253192064342969</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.2421047376459331</c:v>
+                  <c:v>5.4362553651474377</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.2216837901167459</c:v>
+                  <c:v>5.5870042921179497</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.2393470320933968</c:v>
+                  <c:v>5.4886034336943599</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.2344776256747174</c:v>
+                  <c:v>5.4318827469554885</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.2405821005397737</c:v>
+                  <c:v>5.207506197564391</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.2134656804318187</c:v>
+                  <c:v>5.1130049580515129</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.2357725443454557</c:v>
+                  <c:v>5.1564039664412107</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.2536180354763653</c:v>
+                  <c:v>5.0171231731529691</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.2438944283810924</c:v>
+                  <c:v>4.870698538522376</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.2531155427048741</c:v>
+                  <c:v>4.7915588308179009</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.2774924341639</c:v>
+                  <c:v>4.8422470646543214</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.2819939473311202</c:v>
+                  <c:v>4.8297976517234575</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.2665951578648968</c:v>
+                  <c:v>4.8788381213787666</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.2502761262919178</c:v>
+                  <c:v>4.846070497103014</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.2272209010335349</c:v>
+                  <c:v>4.8628563976824113</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.9237767208268277</c:v>
+                  <c:v>4.3842851181459288</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.6850213766614619</c:v>
+                  <c:v>4.3484280945167431</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.4880171013291701</c:v>
+                  <c:v>4.2407424756133949</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.3624136810633365</c:v>
+                  <c:v>3.8585939804907161</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.2699309448506693</c:v>
+                  <c:v>3.8698751843925732</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.1919447558805354</c:v>
+                  <c:v>3.9169001475140588</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.0915558047044289</c:v>
+                  <c:v>3.9055201180112471</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.0122446437635437</c:v>
+                  <c:v>3.7004160944089981</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.9767957150108351</c:v>
+                  <c:v>3.7123328755271983</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.948436572008668</c:v>
+                  <c:v>3.5128663004217588</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.8887492576069347</c:v>
+                  <c:v>3.5532930403374072</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.863999406085548</c:v>
+                  <c:v>3.4286344322699258</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.8591995248684388</c:v>
+                  <c:v>3.5259075458159406</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.8243596198947514</c:v>
+                  <c:v>3.3947260366527523</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.8304876959158012</c:v>
+                  <c:v>3.4647808293222022</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.1403901567326411</c:v>
+                  <c:v>3.9858246634577625</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.3903121253861128</c:v>
+                  <c:v>4.1996597307662098</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.5872497003088908</c:v>
+                  <c:v>4.2327277846129681</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.6907997602471125</c:v>
+                  <c:v>4.525182227690375</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.8086398081976904</c:v>
+                  <c:v>4.6731457821523001</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.8809118465581527</c:v>
+                  <c:v>4.6675166257218406</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.9627294772465227</c:v>
+                  <c:v>4.7560133005774725</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>5.0041835817972187</c:v>
+                  <c:v>4.6858106404619786</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.0463468654377754</c:v>
+                  <c:v>4.877648512369583</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>5.0800774923502203</c:v>
+                  <c:v>5.0941188098956669</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>5.0950619938801758</c:v>
+                  <c:v>5.2632950479165332</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.12004959510414</c:v>
+                  <c:v>5.0846360383332261</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>5.1200396760833122</c:v>
+                  <c:v>5.2917088306665816</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.1410317408666497</c:v>
+                  <c:v>5.3883670645332655</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>5.1438253926933193</c:v>
+                  <c:v>5.4706936516266129</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>5.1650603141546556</c:v>
+                  <c:v>5.613554921301291</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.2080482513237243</c:v>
+                  <c:v>5.5608439370410334</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.2014386010589799</c:v>
+                  <c:v>5.5166751496328263</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.2121508808471839</c:v>
+                  <c:v>5.4653401197062621</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.2377207046777468</c:v>
+                  <c:v>5.4262720957650101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3191,49 +3191,49 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>7</c:v>
@@ -3551,217 +3551,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>3.27</c:v>
+                  <c:v>5.35</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>2.2599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.09</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.59</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>4.2300000000000004</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.94</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.91</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.05</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.64</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.42</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.8600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>3.16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.98</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>5.43</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>3.4</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.58</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3.51</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>3.64</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="20">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>3.16</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>5.38</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>3.19</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>3.41</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>3.38</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.55</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>3.31</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>1.62</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>2.4700000000000002</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>3.66</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.92</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>1.57</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>1.95</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>3.09</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>2.56</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>3.15</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>1.94</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>5.41</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>4.62</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.21</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>4.72</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.76</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.5199999999999996</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.4300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>4.43</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.86</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>4.83</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.74</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>4.49</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>5.14</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>3.11</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1.73</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.3899999999999997</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>3.53</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>2.29</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>3.22</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1.81</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>4.29</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>4.92</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>4.88</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1.74</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>5.24</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>4.55</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>4.5999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>5.37</c:v>
+                </c:pt>
+                <c:pt idx="67">
                   <c:v>3.7</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>3.45</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>3.32</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>3.28</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>3.23</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>3.62</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>3.73</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>3.61</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>3.39</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>3.28</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>3.62</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>3.53</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>3.21</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>3.41</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>3.58</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>3.6</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>3.41</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>3.37</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>3.27</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.42</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.46</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.4</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.72</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.8</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.38</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.39</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.67</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.3</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.53</c:v>
-                </c:pt>
-                <c:pt idx="48">
+                <c:pt idx="68">
                   <c:v>3.68</c:v>
                 </c:pt>
-                <c:pt idx="49">
-                  <c:v>3.37</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3.71</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>3.78</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>3.75</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>3.21</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>3.56</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>3.34</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>3.58</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3.34</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>3.43</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>3.31</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>3.44</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>3.24</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>3.45</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>3.31</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>3.5</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>3.76</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>3.35</c:v>
-                </c:pt>
                 <c:pt idx="69">
-                  <c:v>3.51</c:v>
+                  <c:v>3.52</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3.68</c:v>
+                  <c:v>3.54</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4920,49 +4920,49 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>7</c:v>
@@ -5748,217 +5748,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>5.1349999999999998</c:v>
+                  <c:v>6.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.1479999999999997</c:v>
+                  <c:v>5.8660000000000005</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.1834000000000007</c:v>
+                  <c:v>5.6018000000000008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.2047200000000009</c:v>
+                  <c:v>5.731440000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.2147760000000014</c:v>
+                  <c:v>5.7441520000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.2358208000000017</c:v>
+                  <c:v>5.6243216000000009</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>5.2296566400000017</c:v>
+                  <c:v>5.5894572800000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5.221725312000002</c:v>
+                  <c:v>5.5945658240000009</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.232380249600002</c:v>
+                  <c:v>5.4696526592000003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.2619041996800018</c:v>
+                  <c:v>5.4657221273600003</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.2525233597440018</c:v>
+                  <c:v>5.3915777018880009</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.2330186877952016</c:v>
+                  <c:v>5.4042621615104007</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5.2564149502361621</c:v>
+                  <c:v>5.4284097292083215</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>5.2501319601889298</c:v>
+                  <c:v>5.3067277833666582</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>5.2321055681511437</c:v>
+                  <c:v>5.1873822266933267</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>5.2136844545209158</c:v>
+                  <c:v>5.3359057813546613</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>5.1939475636167334</c:v>
+                  <c:v>5.2847246250837294</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>5.1851580508933868</c:v>
+                  <c:v>5.3257797000669838</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>5.2101264407147099</c:v>
+                  <c:v>5.5036237600535873</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.2411011525717681</c:v>
+                  <c:v>5.4428990080428701</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.253880922057415</c:v>
+                  <c:v>5.5253192064342969</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5.2421047376459331</c:v>
+                  <c:v>5.4362553651474377</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5.2216837901167459</c:v>
+                  <c:v>5.5870042921179497</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.2393470320933968</c:v>
+                  <c:v>5.4886034336943599</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5.2344776256747174</c:v>
+                  <c:v>5.4318827469554885</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5.2405821005397737</c:v>
+                  <c:v>5.207506197564391</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5.2134656804318187</c:v>
+                  <c:v>5.1130049580515129</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5.2357725443454557</c:v>
+                  <c:v>5.1564039664412107</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.2536180354763653</c:v>
+                  <c:v>5.0171231731529691</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.2438944283810924</c:v>
+                  <c:v>4.870698538522376</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5.2531155427048741</c:v>
+                  <c:v>4.7915588308179009</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>5.2774924341639</c:v>
+                  <c:v>4.8422470646543214</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>5.2819939473311202</c:v>
+                  <c:v>4.8297976517234575</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>5.2665951578648968</c:v>
+                  <c:v>4.8788381213787666</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>5.2502761262919178</c:v>
+                  <c:v>4.846070497103014</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.2272209010335349</c:v>
+                  <c:v>4.8628563976824113</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4.9237767208268277</c:v>
+                  <c:v>4.3842851181459288</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4.6850213766614619</c:v>
+                  <c:v>4.3484280945167431</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4.4880171013291701</c:v>
+                  <c:v>4.2407424756133949</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4.3624136810633365</c:v>
+                  <c:v>3.8585939804907161</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.2699309448506693</c:v>
+                  <c:v>3.8698751843925732</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4.1919447558805354</c:v>
+                  <c:v>3.9169001475140588</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4.0915558047044289</c:v>
+                  <c:v>3.9055201180112471</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4.0122446437635437</c:v>
+                  <c:v>3.7004160944089981</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.9767957150108351</c:v>
+                  <c:v>3.7123328755271983</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.948436572008668</c:v>
+                  <c:v>3.5128663004217588</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.8887492576069347</c:v>
+                  <c:v>3.5532930403374072</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.863999406085548</c:v>
+                  <c:v>3.4286344322699258</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.8591995248684388</c:v>
+                  <c:v>3.5259075458159406</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.8243596198947514</c:v>
+                  <c:v>3.3947260366527523</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.8304876959158012</c:v>
+                  <c:v>3.4647808293222022</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>4.1403901567326411</c:v>
+                  <c:v>3.9858246634577625</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>4.3903121253861128</c:v>
+                  <c:v>4.1996597307662098</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>4.5872497003088908</c:v>
+                  <c:v>4.2327277846129681</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.6907997602471125</c:v>
+                  <c:v>4.525182227690375</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>4.8086398081976904</c:v>
+                  <c:v>4.6731457821523001</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>4.8809118465581527</c:v>
+                  <c:v>4.6675166257218406</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.9627294772465227</c:v>
+                  <c:v>4.7560133005774725</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>5.0041835817972187</c:v>
+                  <c:v>4.6858106404619786</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.0463468654377754</c:v>
+                  <c:v>4.877648512369583</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>5.0800774923502203</c:v>
+                  <c:v>5.0941188098956669</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>5.0950619938801758</c:v>
+                  <c:v>5.2632950479165332</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.12004959510414</c:v>
+                  <c:v>5.0846360383332261</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>5.1200396760833122</c:v>
+                  <c:v>5.2917088306665816</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>5.1410317408666497</c:v>
+                  <c:v>5.3883670645332655</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>5.1438253926933193</c:v>
+                  <c:v>5.4706936516266129</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>5.1650603141546556</c:v>
+                  <c:v>5.613554921301291</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.2080482513237243</c:v>
+                  <c:v>5.5608439370410334</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.2014386010589799</c:v>
+                  <c:v>5.5166751496328263</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.2121508808471839</c:v>
+                  <c:v>5.4653401197062621</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.2377207046777468</c:v>
+                  <c:v>5.4262720957650101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6649,49 +6649,49 @@
                   <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>4</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>7</c:v>
@@ -7009,217 +7009,217 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="71"/>
                 <c:pt idx="0">
-                  <c:v>5.1349999999999998</c:v>
+                  <c:v>6.1749999999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>4.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.5449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.25</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.7949999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.1449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>5.6150000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>4.97</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5.45</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>5.0949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>5.4550000000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.5250000000000004</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.82</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.71</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>5.93</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.49</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>6.2149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
                   <c:v>5.2</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>5.2549999999999999</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.32</c:v>
-                </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="20">
+                  <c:v>5.8550000000000004</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>5.08</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>6.1899999999999995</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>5.0949999999999998</c:v>
+                </c:pt>
+                <c:pt idx="24">
                   <c:v>5.2050000000000001</c:v>
                 </c:pt>
-                <c:pt idx="7">
-                  <c:v>5.1899999999999995</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>5.2750000000000004</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.38</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.1550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
+                <c:pt idx="25">
+                  <c:v>4.3100000000000005</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>4.7350000000000003</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>5.33</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>4.46</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>4.2850000000000001</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>4.4749999999999996</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>5.0449999999999999</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>4.78</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>5.0750000000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>4.7149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.93</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>2.4699999999999998</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>4.2050000000000001</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>3.81</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>2.33</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>3.915</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>4.1050000000000004</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>3.86</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>2.88</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>3.76</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>2.7149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>3.7149999999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>2.9299999999999997</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>3.915</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>2.87</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>3.7450000000000001</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>6.07</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>5.0549999999999997</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>4.3650000000000002</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>5.6950000000000003</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>5.2649999999999997</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>4.6449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>5.1100000000000003</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>4.4050000000000002</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>5.6449999999999996</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>5.96</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>5.9399999999999995</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>4.37</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>6.12</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>5.7750000000000004</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.1850000000000005</c:v>
+                </c:pt>
+                <c:pt idx="67">
                   <c:v>5.35</c:v>
                 </c:pt>
-                <c:pt idx="13">
-                  <c:v>5.2249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>5.16</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>5.14</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>5.1150000000000002</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>5.15</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>5.3100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.3650000000000002</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>5.3049999999999997</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>5.1950000000000003</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>5.14</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.3100000000000005</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>5.2649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>5.1050000000000004</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>5.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>5.3250000000000002</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>5.2050000000000001</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>5.375</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>5.3</c:v>
-                </c:pt>
-                <c:pt idx="33">
-                  <c:v>5.2050000000000001</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>5.1850000000000005</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>5.1349999999999998</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>3.71</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>3.73</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>3.7</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>3.8600000000000003</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>3.9</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>3.88</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.69</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>3.6950000000000003</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>3.835</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>3.835</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.65</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.7649999999999997</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3.84</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>3.6850000000000001</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>3.855</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>5.38</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>5.39</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>5.375</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>5.1050000000000004</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>5.28</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>5.17</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>5.29</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.17</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5.2149999999999999</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5.1550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5.22</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5.12</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>5.2249999999999996</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5.1550000000000002</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>5.25</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>5.38</c:v>
-                </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.1749999999999998</c:v>
+                  <c:v>5.34</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.2549999999999999</c:v>
+                  <c:v>5.26</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.34</c:v>
+                  <c:v>5.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -8421,7 +8421,7 @@
   <dimension ref="B1:H74"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S14" sqref="S14"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8439,7 +8439,7 @@
         <v>6</v>
       </c>
       <c r="C1">
-        <v>30</v>
+        <v>200</v>
       </c>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
@@ -8470,16 +8470,16 @@
         <v>7</v>
       </c>
       <c r="E4">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.27</v>
+        <f t="shared" ref="E4:E35" ca="1" si="0">RANDBETWEEN(350-noise,350+noise)/100</f>
+        <v>5.35</v>
       </c>
       <c r="F4">
         <f ca="1">(D4+E4)/2</f>
-        <v>5.1349999999999998</v>
+        <v>6.1749999999999998</v>
       </c>
       <c r="G4">
         <f ca="1">F4</f>
-        <v>5.1349999999999998</v>
+        <v>6.1749999999999998</v>
       </c>
       <c r="H4">
         <v>6</v>
@@ -8493,16 +8493,16 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.4</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.2599999999999998</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F68" ca="1" si="0">(D5+E5)/2</f>
-        <v>5.2</v>
+        <f t="shared" ref="F5:F68" ca="1" si="1">(D5+E5)/2</f>
+        <v>4.63</v>
       </c>
       <c r="G5">
         <f ca="1">G4*0.8+F5*0.2</f>
-        <v>5.1479999999999997</v>
+        <v>5.8660000000000005</v>
       </c>
       <c r="H5">
         <v>6</v>
@@ -8516,16 +8516,16 @@
         <v>7</v>
       </c>
       <c r="E6">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.65</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.09</v>
       </c>
       <c r="F6">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3250000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.5449999999999999</v>
       </c>
       <c r="G6">
-        <f t="shared" ref="G6:G69" ca="1" si="1">G5*0.8+F6*0.2</f>
-        <v>5.1834000000000007</v>
+        <f t="shared" ref="G6:G69" ca="1" si="2">G5*0.8+F6*0.2</f>
+        <v>5.6018000000000008</v>
       </c>
       <c r="H6">
         <v>6</v>
@@ -8539,16 +8539,16 @@
         <v>7</v>
       </c>
       <c r="E7">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.58</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5.5</v>
       </c>
       <c r="F7">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.29</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6.25</v>
       </c>
       <c r="G7">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2047200000000009</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.731440000000001</v>
       </c>
       <c r="H7">
         <v>6</v>
@@ -8562,16 +8562,16 @@
         <v>7</v>
       </c>
       <c r="E8">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.51</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.59</v>
       </c>
       <c r="F8">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2549999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.7949999999999999</v>
       </c>
       <c r="G8">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2147760000000014</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.7441520000000006</v>
       </c>
       <c r="H8">
         <v>6</v>
@@ -8585,16 +8585,16 @@
         <v>7</v>
       </c>
       <c r="E9">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.64</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.29</v>
       </c>
       <c r="F9">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.32</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.1449999999999996</v>
       </c>
       <c r="G9">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2358208000000017</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.6243216000000009</v>
       </c>
       <c r="H9">
         <v>6</v>
@@ -8608,16 +8608,16 @@
         <v>7</v>
       </c>
       <c r="E10">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9</v>
       </c>
       <c r="F10">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2050000000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.45</v>
       </c>
       <c r="G10">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2296566400000017</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.5894572800000004</v>
       </c>
       <c r="H10">
         <v>6</v>
@@ -8631,16 +8631,16 @@
         <v>7</v>
       </c>
       <c r="E11">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.38</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.2300000000000004</v>
       </c>
       <c r="F11">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1899999999999995</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.6150000000000002</v>
       </c>
       <c r="G11">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.221725312000002</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.5945658240000009</v>
       </c>
       <c r="H11">
         <v>6</v>
@@ -8654,16 +8654,16 @@
         <v>7</v>
       </c>
       <c r="E12">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.55</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.94</v>
       </c>
       <c r="F12">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2750000000000004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.97</v>
       </c>
       <c r="G12">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.232380249600002</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4696526592000003</v>
       </c>
       <c r="H12">
         <v>6</v>
@@ -8677,16 +8677,16 @@
         <v>7</v>
       </c>
       <c r="E13">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.76</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.9</v>
       </c>
       <c r="F13">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.38</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.45</v>
       </c>
       <c r="G13">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2619041996800018</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4657221273600003</v>
       </c>
       <c r="H13">
         <v>6</v>
@@ -8700,16 +8700,16 @@
         <v>7</v>
       </c>
       <c r="E14">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.43</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.19</v>
       </c>
       <c r="F14">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2149999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0949999999999998</v>
       </c>
       <c r="G14">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2525233597440018</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.3915777018880009</v>
       </c>
       <c r="H14">
         <v>6</v>
@@ -8723,16 +8723,16 @@
         <v>7</v>
       </c>
       <c r="E15">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.31</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.91</v>
       </c>
       <c r="F15">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1550000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.4550000000000001</v>
       </c>
       <c r="G15">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2330186877952016</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4042621615104007</v>
       </c>
       <c r="H15">
         <v>6</v>
@@ -8746,16 +8746,16 @@
         <v>7</v>
       </c>
       <c r="E16">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.7</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.05</v>
       </c>
       <c r="F16">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.35</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.5250000000000004</v>
       </c>
       <c r="G16">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2564149502361621</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4284097292083215</v>
       </c>
       <c r="H16">
         <v>6</v>
@@ -8769,16 +8769,16 @@
         <v>7</v>
       </c>
       <c r="E17">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.45</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.64</v>
       </c>
       <c r="F17">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2249999999999996</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.82</v>
       </c>
       <c r="G17">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2501319601889298</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.3067277833666582</v>
       </c>
       <c r="H17">
         <v>6</v>
@@ -8792,16 +8792,16 @@
         <v>7</v>
       </c>
       <c r="E18">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.32</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.42</v>
       </c>
       <c r="F18">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.16</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.71</v>
       </c>
       <c r="G18">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2321055681511437</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1873822266933267</v>
       </c>
       <c r="H18">
         <v>6</v>
@@ -8815,16 +8815,16 @@
         <v>7</v>
       </c>
       <c r="E19">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.28</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.8600000000000003</v>
       </c>
       <c r="F19">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.14</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.93</v>
       </c>
       <c r="G19">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2136844545209158</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.3359057813546613</v>
       </c>
       <c r="H19">
         <v>6</v>
@@ -8838,16 +8838,16 @@
         <v>7</v>
       </c>
       <c r="E20">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.23</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.16</v>
       </c>
       <c r="F20">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1150000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.08</v>
       </c>
       <c r="G20">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.1939475636167334</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.2847246250837294</v>
       </c>
       <c r="H20">
         <v>6</v>
@@ -8861,16 +8861,16 @@
         <v>7</v>
       </c>
       <c r="E21">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.3</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.98</v>
       </c>
       <c r="F21">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.15</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.49</v>
       </c>
       <c r="G21">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.1851580508933868</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.3257797000669838</v>
       </c>
       <c r="H21">
         <v>6</v>
@@ -8884,16 +8884,16 @@
         <v>7</v>
       </c>
       <c r="E22">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.62</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5.43</v>
       </c>
       <c r="F22">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3100000000000005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6.2149999999999999</v>
       </c>
       <c r="G22">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2101264407147099</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.5036237600535873</v>
       </c>
       <c r="H22">
         <v>6</v>
@@ -8907,16 +8907,16 @@
         <v>7</v>
       </c>
       <c r="E23">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.73</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.4</v>
       </c>
       <c r="F23">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3650000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.2</v>
       </c>
       <c r="G23">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2411011525717681</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4428990080428701</v>
       </c>
       <c r="H23">
         <v>6</v>
@@ -8930,16 +8930,16 @@
         <v>7</v>
       </c>
       <c r="E24">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.61</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>4.71</v>
       </c>
       <c r="F24">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3049999999999997</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.8550000000000004</v>
       </c>
       <c r="G24">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.253880922057415</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.5253192064342969</v>
       </c>
       <c r="H24">
         <v>6</v>
@@ -8953,16 +8953,16 @@
         <v>7</v>
       </c>
       <c r="E25">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.39</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.16</v>
       </c>
       <c r="F25">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1950000000000003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.08</v>
       </c>
       <c r="G25">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2421047376459331</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4362553651474377</v>
       </c>
       <c r="H25">
         <v>6</v>
@@ -8976,16 +8976,16 @@
         <v>7</v>
       </c>
       <c r="E26">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.28</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>5.38</v>
       </c>
       <c r="F26">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.14</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6.1899999999999995</v>
       </c>
       <c r="G26">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2216837901167459</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.5870042921179497</v>
       </c>
       <c r="H26">
         <v>6</v>
@@ -8999,16 +8999,16 @@
         <v>7</v>
       </c>
       <c r="E27">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.62</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.19</v>
       </c>
       <c r="F27">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3100000000000005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0949999999999998</v>
       </c>
       <c r="G27">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2393470320933968</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4886034336943599</v>
       </c>
       <c r="H27">
         <v>6</v>
@@ -9022,16 +9022,16 @@
         <v>7</v>
       </c>
       <c r="E28">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.43</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.41</v>
       </c>
       <c r="F28">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2149999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.2050000000000001</v>
       </c>
       <c r="G28">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2344776256747174</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4318827469554885</v>
       </c>
       <c r="H28">
         <v>6</v>
@@ -9045,16 +9045,16 @@
         <v>7</v>
       </c>
       <c r="E29">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.53</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.62</v>
       </c>
       <c r="F29">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2649999999999997</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.3100000000000005</v>
       </c>
       <c r="G29">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2405821005397737</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.207506197564391</v>
       </c>
       <c r="H29">
         <v>6</v>
@@ -9068,16 +9068,16 @@
         <v>7</v>
       </c>
       <c r="E30">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.21</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>2.4700000000000002</v>
       </c>
       <c r="F30">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1050000000000004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.7350000000000003</v>
       </c>
       <c r="G30">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2134656804318187</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1130049580515129</v>
       </c>
       <c r="H30">
         <v>6</v>
@@ -9091,16 +9091,16 @@
         <v>7</v>
       </c>
       <c r="E31">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.65</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.66</v>
       </c>
       <c r="F31">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3250000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.33</v>
       </c>
       <c r="G31">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2357725443454557</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.1564039664412107</v>
       </c>
       <c r="H31">
         <v>6</v>
@@ -9114,16 +9114,16 @@
         <v>7</v>
       </c>
       <c r="E32">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.65</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.92</v>
       </c>
       <c r="F32">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3250000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.46</v>
       </c>
       <c r="G32">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2536180354763653</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0171231731529691</v>
       </c>
       <c r="H32">
         <v>6</v>
@@ -9137,16 +9137,16 @@
         <v>7</v>
       </c>
       <c r="E33">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.41</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.57</v>
       </c>
       <c r="F33">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2050000000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.2850000000000001</v>
       </c>
       <c r="G33">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2438944283810924</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.870698538522376</v>
       </c>
       <c r="H33">
         <v>6</v>
@@ -9160,16 +9160,16 @@
         <v>7</v>
       </c>
       <c r="E34">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.58</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>1.95</v>
       </c>
       <c r="F34">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.29</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.4749999999999996</v>
       </c>
       <c r="G34">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2531155427048741</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.7915588308179009</v>
       </c>
       <c r="H34">
         <v>6</v>
@@ -9183,16 +9183,16 @@
         <v>7</v>
       </c>
       <c r="E35">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.75</v>
+        <f t="shared" ca="1" si="0"/>
+        <v>3.09</v>
       </c>
       <c r="F35">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.375</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0449999999999999</v>
       </c>
       <c r="G35">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2774924341639</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8422470646543214</v>
       </c>
       <c r="H35">
         <v>6</v>
@@ -9206,16 +9206,16 @@
         <v>7</v>
       </c>
       <c r="E36">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.6</v>
+        <f t="shared" ref="E36:E67" ca="1" si="3">RANDBETWEEN(350-noise,350+noise)/100</f>
+        <v>2.56</v>
       </c>
       <c r="F36">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.3</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.78</v>
       </c>
       <c r="G36">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2819939473311202</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8297976517234575</v>
       </c>
       <c r="H36">
         <v>6</v>
@@ -9229,16 +9229,16 @@
         <v>7</v>
       </c>
       <c r="E37">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.41</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3.15</v>
       </c>
       <c r="F37">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2050000000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0750000000000002</v>
       </c>
       <c r="G37">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2665951578648968</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8788381213787666</v>
       </c>
       <c r="H37">
         <v>6</v>
@@ -9252,16 +9252,16 @@
         <v>7</v>
       </c>
       <c r="E38">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.37</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="F38">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1850000000000005</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.7149999999999999</v>
       </c>
       <c r="G38">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2502761262919178</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.846070497103014</v>
       </c>
       <c r="H38">
         <v>6</v>
@@ -9275,16 +9275,16 @@
         <v>7</v>
       </c>
       <c r="E39">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.27</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.86</v>
       </c>
       <c r="F39">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1349999999999998</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.93</v>
       </c>
       <c r="G39">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.2272209010335349</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.8628563976824113</v>
       </c>
       <c r="H39">
         <v>6</v>
@@ -9295,19 +9295,19 @@
         <v>1.8</v>
       </c>
       <c r="D40">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E40">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.42</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.94</v>
       </c>
       <c r="F40">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.71</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.4699999999999998</v>
       </c>
       <c r="G40">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.9237767208268277</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.3842851181459288</v>
       </c>
       <c r="H40">
         <v>6</v>
@@ -9318,19 +9318,19 @@
         <v>1.85</v>
       </c>
       <c r="D41">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E41">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.46</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5.41</v>
       </c>
       <c r="F41">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.73</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.2050000000000001</v>
       </c>
       <c r="G41">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.6850213766614619</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.3484280945167431</v>
       </c>
       <c r="H41">
         <v>6</v>
@@ -9341,19 +9341,19 @@
         <v>1.9</v>
       </c>
       <c r="D42">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E42">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.4</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.62</v>
       </c>
       <c r="F42">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.81</v>
       </c>
       <c r="G42">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.4880171013291701</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.2407424756133949</v>
       </c>
       <c r="H42">
         <v>6</v>
@@ -9364,19 +9364,19 @@
         <v>1.95</v>
       </c>
       <c r="D43">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E43">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.72</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.66</v>
       </c>
       <c r="F43">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.8600000000000003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.33</v>
       </c>
       <c r="G43">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.3624136810633365</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.8585939804907161</v>
       </c>
       <c r="H43">
         <v>6</v>
@@ -9387,19 +9387,19 @@
         <v>2</v>
       </c>
       <c r="D44">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E44">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.8</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.83</v>
       </c>
       <c r="F44">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.9</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.915</v>
       </c>
       <c r="G44">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.2699309448506693</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.8698751843925732</v>
       </c>
       <c r="H44">
         <v>6</v>
@@ -9410,19 +9410,19 @@
         <v>2.0499999999999998</v>
       </c>
       <c r="D45">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E45">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.76</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5.21</v>
       </c>
       <c r="F45">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.88</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.1050000000000004</v>
       </c>
       <c r="G45">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.1919447558805354</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.9169001475140588</v>
       </c>
       <c r="H45">
         <v>6</v>
@@ -9433,19 +9433,19 @@
         <v>2.1</v>
       </c>
       <c r="D46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E46">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.38</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.72</v>
       </c>
       <c r="F46">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.69</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.86</v>
       </c>
       <c r="G46">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.0915558047044289</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.9055201180112471</v>
       </c>
       <c r="H46">
         <v>6</v>
@@ -9456,19 +9456,19 @@
         <v>2.15</v>
       </c>
       <c r="D47">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E47">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.39</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.76</v>
       </c>
       <c r="F47">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.6950000000000003</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.88</v>
       </c>
       <c r="G47">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.0122446437635437</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.7004160944089981</v>
       </c>
       <c r="H47">
         <v>6</v>
@@ -9479,19 +9479,19 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="D48">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E48">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.67</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.5199999999999996</v>
       </c>
       <c r="F48">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.835</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.76</v>
       </c>
       <c r="G48">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.9767957150108351</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.7123328755271983</v>
       </c>
       <c r="H48">
         <v>6</v>
@@ -9502,19 +9502,19 @@
         <v>2.25</v>
       </c>
       <c r="D49">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E49">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.67</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.4300000000000002</v>
       </c>
       <c r="F49">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.835</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.7149999999999999</v>
       </c>
       <c r="G49">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.948436572008668</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.5128663004217588</v>
       </c>
       <c r="H49">
         <v>6</v>
@@ -9525,19 +9525,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D50">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E50">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.3</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.43</v>
       </c>
       <c r="F50">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.65</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.7149999999999999</v>
       </c>
       <c r="G50">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.8887492576069347</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.5532930403374072</v>
       </c>
       <c r="H50">
         <v>6</v>
@@ -9548,19 +9548,19 @@
         <v>2.35</v>
       </c>
       <c r="D51">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E51">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.53</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.86</v>
       </c>
       <c r="F51">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.7649999999999997</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.9299999999999997</v>
       </c>
       <c r="G51">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.863999406085548</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.4286344322699258</v>
       </c>
       <c r="H51">
         <v>6</v>
@@ -9571,19 +9571,19 @@
         <v>2.4</v>
       </c>
       <c r="D52">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E52">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.68</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.83</v>
       </c>
       <c r="F52">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.84</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.915</v>
       </c>
       <c r="G52">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.8591995248684388</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.5259075458159406</v>
       </c>
       <c r="H52">
         <v>6</v>
@@ -9594,19 +9594,19 @@
         <v>2.4500000000000002</v>
       </c>
       <c r="D53">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E53">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.37</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.74</v>
       </c>
       <c r="F53">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.6850000000000001</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>2.87</v>
       </c>
       <c r="G53">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.8243596198947514</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.3947260366527523</v>
       </c>
       <c r="H53">
         <v>6</v>
@@ -9617,19 +9617,19 @@
         <v>2.5</v>
       </c>
       <c r="D54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="E54">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.71</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.49</v>
       </c>
       <c r="F54">
-        <f t="shared" ca="1" si="0"/>
-        <v>3.855</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>3.7450000000000001</v>
       </c>
       <c r="G54">
-        <f t="shared" ca="1" si="1"/>
-        <v>3.8304876959158012</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.4647808293222022</v>
       </c>
       <c r="H54">
         <v>6</v>
@@ -9643,16 +9643,16 @@
         <v>7</v>
       </c>
       <c r="E55">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.76</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5.14</v>
       </c>
       <c r="F55">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.38</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6.07</v>
       </c>
       <c r="G55">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.1403901567326411</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>3.9858246634577625</v>
       </c>
       <c r="H55">
         <v>6</v>
@@ -9666,16 +9666,16 @@
         <v>7</v>
       </c>
       <c r="E56">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.78</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3.11</v>
       </c>
       <c r="F56">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.39</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.0549999999999997</v>
       </c>
       <c r="G56">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.3903121253861128</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.1996597307662098</v>
       </c>
       <c r="H56">
         <v>6</v>
@@ -9689,16 +9689,16 @@
         <v>7</v>
       </c>
       <c r="E57">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.75</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.73</v>
       </c>
       <c r="F57">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.375</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.3650000000000002</v>
       </c>
       <c r="G57">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.5872497003088908</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.2327277846129681</v>
       </c>
       <c r="H57">
         <v>6</v>
@@ -9712,16 +9712,16 @@
         <v>7</v>
       </c>
       <c r="E58">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.21</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.3899999999999997</v>
       </c>
       <c r="F58">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1050000000000004</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.6950000000000003</v>
       </c>
       <c r="G58">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.6907997602471125</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.525182227690375</v>
       </c>
       <c r="H58">
         <v>6</v>
@@ -9735,16 +9735,16 @@
         <v>7</v>
       </c>
       <c r="E59">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.56</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3.53</v>
       </c>
       <c r="F59">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.28</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.2649999999999997</v>
       </c>
       <c r="G59">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.8086398081976904</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.6731457821523001</v>
       </c>
       <c r="H59">
         <v>6</v>
@@ -9758,16 +9758,16 @@
         <v>7</v>
       </c>
       <c r="E60">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.34</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>2.29</v>
       </c>
       <c r="F60">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.17</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.6449999999999996</v>
       </c>
       <c r="G60">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.8809118465581527</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.6675166257218406</v>
       </c>
       <c r="H60">
         <v>6</v>
@@ -9781,16 +9781,16 @@
         <v>7</v>
       </c>
       <c r="E61">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.58</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>3.22</v>
       </c>
       <c r="F61">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.29</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.1100000000000003</v>
       </c>
       <c r="G61">
-        <f t="shared" ca="1" si="1"/>
-        <v>4.9627294772465227</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.7560133005774725</v>
       </c>
       <c r="H61">
         <v>6</v>
@@ -9804,16 +9804,16 @@
         <v>7</v>
       </c>
       <c r="E62">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.34</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.81</v>
       </c>
       <c r="F62">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.17</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.4050000000000002</v>
       </c>
       <c r="G62">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.0041835817972187</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.6858106404619786</v>
       </c>
       <c r="H62">
         <v>6</v>
@@ -9827,16 +9827,16 @@
         <v>7</v>
       </c>
       <c r="E63">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.43</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.29</v>
       </c>
       <c r="F63">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2149999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.6449999999999996</v>
       </c>
       <c r="G63">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.0463468654377754</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>4.877648512369583</v>
       </c>
       <c r="H63">
         <v>6</v>
@@ -9850,16 +9850,16 @@
         <v>7</v>
       </c>
       <c r="E64">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.43</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.92</v>
       </c>
       <c r="F64">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2149999999999999</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.96</v>
       </c>
       <c r="G64">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.0800774923502203</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0941188098956669</v>
       </c>
       <c r="H64">
         <v>6</v>
@@ -9873,16 +9873,16 @@
         <v>7</v>
       </c>
       <c r="E65">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.31</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>4.88</v>
       </c>
       <c r="F65">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.1550000000000002</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.9399999999999995</v>
       </c>
       <c r="G65">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.0950619938801758</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.2632950479165332</v>
       </c>
       <c r="H65">
         <v>6</v>
@@ -9896,16 +9896,16 @@
         <v>7</v>
       </c>
       <c r="E66">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.44</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>1.74</v>
       </c>
       <c r="F66">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.22</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>4.37</v>
       </c>
       <c r="G66">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.12004959510414</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.0846360383332261</v>
       </c>
       <c r="H66">
         <v>6</v>
@@ -9919,16 +9919,16 @@
         <v>7</v>
       </c>
       <c r="E67">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.24</v>
+        <f t="shared" ca="1" si="3"/>
+        <v>5.24</v>
       </c>
       <c r="F67">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.12</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>6.12</v>
       </c>
       <c r="G67">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.1200396760833122</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.2917088306665816</v>
       </c>
       <c r="H67">
         <v>6</v>
@@ -9942,16 +9942,16 @@
         <v>7</v>
       </c>
       <c r="E68">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.45</v>
+        <f t="shared" ref="E68:E74" ca="1" si="4">RANDBETWEEN(350-noise,350+noise)/100</f>
+        <v>4.55</v>
       </c>
       <c r="F68">
-        <f t="shared" ca="1" si="0"/>
-        <v>5.2249999999999996</v>
+        <f t="shared" ca="1" si="1"/>
+        <v>5.7750000000000004</v>
       </c>
       <c r="G68">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.1410317408666497</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.3883670645332655</v>
       </c>
       <c r="H68">
         <v>6</v>
@@ -9965,16 +9965,16 @@
         <v>7</v>
       </c>
       <c r="E69">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.31</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F69">
-        <f t="shared" ref="F69:F74" ca="1" si="2">(D69+E69)/2</f>
-        <v>5.1550000000000002</v>
+        <f t="shared" ref="F69:F74" ca="1" si="5">(D69+E69)/2</f>
+        <v>5.8</v>
       </c>
       <c r="G69">
-        <f t="shared" ca="1" si="1"/>
-        <v>5.1438253926933193</v>
+        <f t="shared" ca="1" si="2"/>
+        <v>5.4706936516266129</v>
       </c>
       <c r="H69">
         <v>6</v>
@@ -9988,16 +9988,16 @@
         <v>7</v>
       </c>
       <c r="E70">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.5</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>5.37</v>
       </c>
       <c r="F70">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.25</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>6.1850000000000005</v>
       </c>
       <c r="G70">
-        <f t="shared" ref="G70:G74" ca="1" si="3">G69*0.8+F70*0.2</f>
-        <v>5.1650603141546556</v>
+        <f t="shared" ref="G70:G74" ca="1" si="6">G69*0.8+F70*0.2</f>
+        <v>5.613554921301291</v>
       </c>
       <c r="H70">
         <v>6</v>
@@ -10011,16 +10011,16 @@
         <v>7</v>
       </c>
       <c r="E71">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.76</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.7</v>
       </c>
       <c r="F71">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.38</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5.35</v>
       </c>
       <c r="G71">
-        <f t="shared" ca="1" si="3"/>
-        <v>5.2080482513237243</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5.5608439370410334</v>
       </c>
       <c r="H71">
         <v>6</v>
@@ -10034,16 +10034,16 @@
         <v>7</v>
       </c>
       <c r="E72">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.35</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.68</v>
       </c>
       <c r="F72">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.1749999999999998</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5.34</v>
       </c>
       <c r="G72">
-        <f t="shared" ca="1" si="3"/>
-        <v>5.2014386010589799</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5.5166751496328263</v>
       </c>
       <c r="H72">
         <v>6</v>
@@ -10057,16 +10057,16 @@
         <v>7</v>
       </c>
       <c r="E73">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.51</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.52</v>
       </c>
       <c r="F73">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.2549999999999999</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5.26</v>
       </c>
       <c r="G73">
-        <f t="shared" ca="1" si="3"/>
-        <v>5.2121508808471839</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5.4653401197062621</v>
       </c>
       <c r="H73">
         <v>6</v>
@@ -10080,16 +10080,16 @@
         <v>7</v>
       </c>
       <c r="E74">
-        <f ca="1">RANDBETWEEN(350-noise,350+noise)/100</f>
-        <v>3.68</v>
+        <f t="shared" ca="1" si="4"/>
+        <v>3.54</v>
       </c>
       <c r="F74">
-        <f t="shared" ca="1" si="2"/>
-        <v>5.34</v>
+        <f t="shared" ca="1" si="5"/>
+        <v>5.27</v>
       </c>
       <c r="G74">
-        <f t="shared" ca="1" si="3"/>
-        <v>5.2377207046777468</v>
+        <f t="shared" ca="1" si="6"/>
+        <v>5.4262720957650101</v>
       </c>
       <c r="H74">
         <v>6</v>

</xml_diff>